<commit_message>
adds min/max for waterVel in trap column and validates xml
</commit_message>
<xml_diff>
--- a/data-raw/metadata/yuba_trap_metadata.xlsx
+++ b/data-raw/metadata/yuba_trap_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashleyvizek/code/jpe-yuba-edi/data-raw/metadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-yuba-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39F2550E-BD8E-CA4E-85E0-9E9A98B032E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33FE1A5A-8C06-EB4F-86CD-053FB64AF074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="62420" yWindow="1560" windowWidth="34120" windowHeight="17980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -547,8 +547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1142,8 +1142,12 @@
       <c r="I14" s="11"/>
       <c r="J14" s="12"/>
       <c r="K14" s="11"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
+      <c r="L14" s="12">
+        <v>0</v>
+      </c>
+      <c r="M14" s="12">
+        <v>0</v>
+      </c>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>

</xml_diff>